<commit_message>
fixbug kal001 :#107522 , 107524 , 107526 , 107529 , 107530
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KAL001-アラームリスト(個人別).xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KAL001-アラームリスト(個人別).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13845" windowHeight="6075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21765" windowHeight="10755"/>
   </bookViews>
   <sheets>
     <sheet name="帳票テンプレート" sheetId="2" r:id="rId1"/>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>社員コード</t>
     <rPh sb="0" eb="2">
@@ -285,10 +285,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>コメント</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>職場名</t>
     <rPh sb="0" eb="2">
       <t>ショクバ</t>
@@ -321,6 +317,15 @@
   </si>
   <si>
     <t>&amp;=item.comment</t>
+  </si>
+  <si>
+    <t>チェック対象値</t>
+  </si>
+  <si>
+    <t>&amp;=item.checkedValue</t>
+  </si>
+  <si>
+    <t>コメント</t>
   </si>
 </sst>
 </file>
@@ -44005,7 +44010,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -44013,9 +44018,10 @@
     <col min="1" max="1" width="12.42578125" style="2" customWidth="1"/>
     <col min="2" max="5" width="10.5703125" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35" style="2" customWidth="1"/>
-    <col min="8" max="8" width="37" style="2" customWidth="1"/>
-    <col min="9" max="11" width="12.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="12.5703125" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -44031,7 +44037,7 @@
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -44052,33 +44058,39 @@
         <v>5</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="36" customHeight="1">
       <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1"/>

</xml_diff>